<commit_message>
si terminado e concavidade fracionada começada
</commit_message>
<xml_diff>
--- a/Python/Toy.xlsx
+++ b/Python/Toy.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Rodrigo S. Hirama\Documentos\EACH\IC\Classification-of-mammography-images\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895A6B7F-D4B9-4BF7-8E7F-35D2CC403253}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167CFCC8-3502-4540-A2AA-568C7B22DEF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="0.05" sheetId="2" r:id="rId1"/>
-    <sheet name="0.01" sheetId="3" r:id="rId2"/>
+    <sheet name="0.01" sheetId="6" r:id="rId1"/>
+    <sheet name="0.05" sheetId="5" r:id="rId2"/>
     <sheet name="0.001" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -453,11 +453,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CC27D4-BC1A-4DD9-B151-064A6B1BB0B2}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,10 +478,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.21460188777366429</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -489,10 +489,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.28142976233338929</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>1.0248730986010499</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -500,10 +500,10 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.45576762036525509</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>1.192010606287883</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,10 +511,10 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.6169617082151404</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>1.491310064922033</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -522,10 +522,10 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.58241811994052517</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1.5639628417602689</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,10 +533,10 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0.46158032993403392</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>1.120785148306801</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -544,10 +544,10 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>0.38880328070452119</v>
+        <v>3</v>
       </c>
       <c r="C8">
-        <v>0.95966091692873678</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,10 +555,10 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0.23779593930082299</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>1.005770839737947</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -566,10 +566,10 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>0.23761519271515369</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>1.006184008993606</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -577,10 +577,10 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.22830972350979639</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>1.014412570148955</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -588,10 +588,10 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>0.22830972350979639</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>1.014412570148955</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -599,10 +599,10 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>0.2260311707577953</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>1.01288357138471</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -610,10 +610,10 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>0.44166818972781419</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1.5070293030406161</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,10 +621,10 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>0.42354810388697212</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>1.4970101799360931</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -632,10 +632,10 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>0.42651604624713851</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>1.4959353471047561</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>-16</v>
       </c>
     </row>
   </sheetData>
@@ -655,11 +655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A56BE110-29F5-41DE-B677-CF66F772C1B6}">
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,10 +680,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>1.3548677635081829E-2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>7.6683975856266684E-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,10 +691,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.17217320065749919</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0.39364417089283499</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -702,10 +702,10 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.35535619745645358</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0.69908080308408638</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,10 +713,10 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.50084184935611109</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>0.97117782266921704</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -724,10 +724,10 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.54732867370911475</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>1.2455556704806501</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -735,10 +735,10 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0.62470722599409978</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>1.3353843424592899</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -746,10 +746,10 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>0.68622929895712026</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>1.2274083263819551</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -757,10 +757,10 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0.72892378597985119</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>1.296999476826739</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -768,10 +768,10 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>0.75216393224395617</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>1.3587230411571241</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -779,10 +779,10 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.80996942264630767</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>1.4414663443946529</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,10 +790,10 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>0.86038295455805358</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>1.561641872018646</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -801,10 +801,10 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>0.89647204317619822</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>1.6449284782361131</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -812,10 +812,10 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>0.9182933149607424</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1.7183929911122651</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,10 +823,10 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>0.93849380538387273</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>1.7772515162704901</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -834,10 +834,10 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>0.94949316812498108</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>1.816284067914405</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -845,10 +845,10 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>0.95417484678207254</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>1.8616471892158131</v>
+        <v>-16</v>
       </c>
     </row>
   </sheetData>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="A1:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,10 +882,10 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>6.3990641180733498E-2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>0.23080247252590841</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -893,10 +893,10 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.20369401358188299</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>0.1334177953312565</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -904,10 +904,10 @@
         <v>11</v>
       </c>
       <c r="B4">
-        <v>0.36793200390824249</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>0.11060446329432751</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -915,10 +915,10 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <v>0.50527384877475923</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>0.19712792907320009</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -926,10 +926,10 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.56495174385537383</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>0.75145789629139559</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -937,10 +937,10 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>0.63099702692163395</v>
+        <v>6</v>
       </c>
       <c r="C7">
-        <v>0.89021726302108595</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -948,10 +948,10 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>0.68731732116997313</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>1.071164327204897</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -959,10 +959,10 @@
         <v>16</v>
       </c>
       <c r="B9">
-        <v>0.73127358128292919</v>
+        <v>8</v>
       </c>
       <c r="C9">
-        <v>1.14255845807768</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -970,10 +970,10 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>0.75905381464699817</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>1.091161851081498</v>
+        <v>-9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -981,10 +981,10 @@
         <v>18</v>
       </c>
       <c r="B11">
-        <v>0.81918187024386002</v>
+        <v>10</v>
       </c>
       <c r="C11">
-        <v>1.165229050193225</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,10 +992,10 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>0.89961123402203391</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>1.136389335367842</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,10 +1003,10 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <v>0.92695531247244212</v>
+        <v>12</v>
       </c>
       <c r="C13">
-        <v>1.1357269232549081</v>
+        <v>-12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1014,10 +1014,10 @@
         <v>7</v>
       </c>
       <c r="B14">
-        <v>0.95203170909832924</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>1.173170136962544</v>
+        <v>-13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1025,10 +1025,10 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>0.95983762052374755</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>1.214102634380605</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1036,10 +1036,10 @@
         <v>9</v>
       </c>
       <c r="B16">
-        <v>0.96500644226157684</v>
+        <v>15</v>
       </c>
       <c r="C16">
-        <v>1.2831896474054629</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1047,10 +1047,10 @@
         <v>10</v>
       </c>
       <c r="B17">
-        <v>0.96988376604104565</v>
+        <v>16</v>
       </c>
       <c r="C17">
-        <v>1.287946044704029</v>
+        <v>-16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>